<commit_message>
ignore UpperCase charactors in query and while NLU parsing
</commit_message>
<xml_diff>
--- a/src/SmartKG.DataProcessor/Resources/_DataPreProcess/excel/COVID19/SmartKG_KGDesc_virsus.xlsx
+++ b/src/SmartKG.DataProcessor/Resources/_DataPreProcess/excel/COVID19/SmartKG_KGDesc_virsus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jull\source\repos\KGBot\DataProcessor\Resources\COVID19\PreProcess\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jull\source\repos\SmartKG\src\SmartKG.DataProcessor\Resources\_DataPreProcess\excel\COVID19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8309BF37-32B1-4F4E-AD69-FAD8588A3FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322CCACB-8B56-434A-8744-358FC92D1AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{3F61220E-6DF8-45A4-8ACE-BD2E47FB9DB7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="252">
   <si>
     <t>实体id</t>
   </si>
@@ -981,6 +981,12 @@
   </si>
   <si>
     <t>预防手段有：</t>
+  </si>
+  <si>
+    <t>COVID-19抗体</t>
+  </si>
+  <si>
+    <t>COVID-19疫苗</t>
   </si>
 </sst>
 </file>
@@ -1343,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E4FB99-2BF2-4C79-8D90-66D366EC24EB}">
   <dimension ref="A1:BF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1720,10 +1726,10 @@
         <v>79</v>
       </c>
       <c r="AV2" t="s">
-        <v>116</v>
+        <v>250</v>
       </c>
       <c r="AW2" t="s">
-        <v>117</v>
+        <v>251</v>
       </c>
       <c r="AX2" t="s">
         <v>88</v>
@@ -2665,7 +2671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9872B5-37CE-4807-88A4-6CEF7C770DDE}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>

</xml_diff>